<commit_message>
update bom kp function
</commit_message>
<xml_diff>
--- a/Assy_Bom/Template/Template.xlsx
+++ b/Assy_Bom/Template/Template.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\CTTV\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="U:\TRSH-PROGRAM\Assy_Bom\Assy_Bom\Template\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -80,8 +80,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -364,9 +365,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="4" max="5" width="8.88671875" style="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
@@ -378,10 +384,10 @@
       <c r="C1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
       <c r="F1" t="s">

</xml_diff>